<commit_message>
the new workbook has been created and is almost ready to use
</commit_message>
<xml_diff>
--- a/venv/modified_file.xlsx
+++ b/venv/modified_file.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q149"/>
+  <dimension ref="A1:M149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,26 +490,6 @@
           <t>year</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Unnamed: 24</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Unnamed: 25</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Unnamed: 26</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Unnamed: 27</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -565,18 +545,6 @@
       <c r="M2" t="n">
         <v>2023</v>
       </c>
-      <c r="N2" t="n">
-        <v/>
-      </c>
-      <c r="O2" t="n">
-        <v/>
-      </c>
-      <c r="P2" t="n">
-        <v/>
-      </c>
-      <c r="Q2" t="n">
-        <v/>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -632,18 +600,6 @@
       <c r="M3" t="n">
         <v>2023</v>
       </c>
-      <c r="N3" t="n">
-        <v/>
-      </c>
-      <c r="O3" t="n">
-        <v/>
-      </c>
-      <c r="P3" t="n">
-        <v/>
-      </c>
-      <c r="Q3" t="n">
-        <v/>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -699,18 +655,6 @@
       <c r="M4" t="n">
         <v>2023</v>
       </c>
-      <c r="N4" t="n">
-        <v/>
-      </c>
-      <c r="O4" t="n">
-        <v/>
-      </c>
-      <c r="P4" t="n">
-        <v/>
-      </c>
-      <c r="Q4" t="n">
-        <v/>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -766,18 +710,6 @@
       <c r="M5" t="n">
         <v>2023</v>
       </c>
-      <c r="N5" t="n">
-        <v/>
-      </c>
-      <c r="O5" t="n">
-        <v/>
-      </c>
-      <c r="P5" t="n">
-        <v/>
-      </c>
-      <c r="Q5" t="n">
-        <v/>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -833,18 +765,6 @@
       <c r="M6" t="n">
         <v>2023</v>
       </c>
-      <c r="N6" t="n">
-        <v/>
-      </c>
-      <c r="O6" t="n">
-        <v/>
-      </c>
-      <c r="P6" t="n">
-        <v/>
-      </c>
-      <c r="Q6" t="n">
-        <v/>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -900,18 +820,6 @@
       <c r="M7" t="n">
         <v>2023</v>
       </c>
-      <c r="N7" t="n">
-        <v/>
-      </c>
-      <c r="O7" t="n">
-        <v/>
-      </c>
-      <c r="P7" t="n">
-        <v/>
-      </c>
-      <c r="Q7" t="n">
-        <v/>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -967,18 +875,6 @@
       <c r="M8" t="n">
         <v>2023</v>
       </c>
-      <c r="N8" t="n">
-        <v/>
-      </c>
-      <c r="O8" t="n">
-        <v/>
-      </c>
-      <c r="P8" t="n">
-        <v/>
-      </c>
-      <c r="Q8" t="n">
-        <v/>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1034,18 +930,6 @@
       <c r="M9" t="n">
         <v>2023</v>
       </c>
-      <c r="N9" t="n">
-        <v/>
-      </c>
-      <c r="O9" t="n">
-        <v/>
-      </c>
-      <c r="P9" t="n">
-        <v/>
-      </c>
-      <c r="Q9" t="n">
-        <v/>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1101,18 +985,6 @@
       <c r="M10" t="n">
         <v>2023</v>
       </c>
-      <c r="N10" t="n">
-        <v/>
-      </c>
-      <c r="O10" t="n">
-        <v/>
-      </c>
-      <c r="P10" t="n">
-        <v/>
-      </c>
-      <c r="Q10" t="n">
-        <v/>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1168,18 +1040,6 @@
       <c r="M11" t="n">
         <v>2023</v>
       </c>
-      <c r="N11" t="n">
-        <v/>
-      </c>
-      <c r="O11" t="n">
-        <v/>
-      </c>
-      <c r="P11" t="n">
-        <v/>
-      </c>
-      <c r="Q11" t="n">
-        <v/>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1235,18 +1095,6 @@
       <c r="M12" t="n">
         <v>2023</v>
       </c>
-      <c r="N12" t="n">
-        <v/>
-      </c>
-      <c r="O12" t="n">
-        <v/>
-      </c>
-      <c r="P12" t="n">
-        <v/>
-      </c>
-      <c r="Q12" t="n">
-        <v/>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1302,18 +1150,6 @@
       <c r="M13" t="n">
         <v>2022</v>
       </c>
-      <c r="N13" t="n">
-        <v/>
-      </c>
-      <c r="O13" t="n">
-        <v/>
-      </c>
-      <c r="P13" t="n">
-        <v/>
-      </c>
-      <c r="Q13" t="n">
-        <v/>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1369,18 +1205,6 @@
       <c r="M14" t="n">
         <v>2022</v>
       </c>
-      <c r="N14" t="n">
-        <v/>
-      </c>
-      <c r="O14" t="n">
-        <v/>
-      </c>
-      <c r="P14" t="n">
-        <v/>
-      </c>
-      <c r="Q14" t="n">
-        <v/>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1436,18 +1260,6 @@
       <c r="M15" t="n">
         <v>2022</v>
       </c>
-      <c r="N15" t="n">
-        <v/>
-      </c>
-      <c r="O15" t="n">
-        <v/>
-      </c>
-      <c r="P15" t="n">
-        <v/>
-      </c>
-      <c r="Q15" t="n">
-        <v/>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1503,18 +1315,6 @@
       <c r="M16" t="n">
         <v>2022</v>
       </c>
-      <c r="N16" t="n">
-        <v/>
-      </c>
-      <c r="O16" t="n">
-        <v/>
-      </c>
-      <c r="P16" t="n">
-        <v/>
-      </c>
-      <c r="Q16" t="n">
-        <v/>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1570,18 +1370,6 @@
       <c r="M17" t="n">
         <v>2022</v>
       </c>
-      <c r="N17" t="n">
-        <v/>
-      </c>
-      <c r="O17" t="n">
-        <v/>
-      </c>
-      <c r="P17" t="n">
-        <v/>
-      </c>
-      <c r="Q17" t="n">
-        <v/>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1637,18 +1425,6 @@
       <c r="M18" t="n">
         <v>2022</v>
       </c>
-      <c r="N18" t="n">
-        <v/>
-      </c>
-      <c r="O18" t="n">
-        <v/>
-      </c>
-      <c r="P18" t="n">
-        <v/>
-      </c>
-      <c r="Q18" t="n">
-        <v/>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1704,18 +1480,6 @@
       <c r="M19" t="n">
         <v>2022</v>
       </c>
-      <c r="N19" t="n">
-        <v/>
-      </c>
-      <c r="O19" t="n">
-        <v/>
-      </c>
-      <c r="P19" t="n">
-        <v/>
-      </c>
-      <c r="Q19" t="n">
-        <v/>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1771,18 +1535,6 @@
       <c r="M20" t="n">
         <v>2022</v>
       </c>
-      <c r="N20" t="n">
-        <v/>
-      </c>
-      <c r="O20" t="n">
-        <v/>
-      </c>
-      <c r="P20" t="n">
-        <v/>
-      </c>
-      <c r="Q20" t="n">
-        <v/>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1838,18 +1590,6 @@
       <c r="M21" t="n">
         <v>2022</v>
       </c>
-      <c r="N21" t="n">
-        <v/>
-      </c>
-      <c r="O21" t="n">
-        <v/>
-      </c>
-      <c r="P21" t="n">
-        <v/>
-      </c>
-      <c r="Q21" t="n">
-        <v/>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1905,18 +1645,6 @@
       <c r="M22" t="n">
         <v>2022</v>
       </c>
-      <c r="N22" t="n">
-        <v/>
-      </c>
-      <c r="O22" t="n">
-        <v/>
-      </c>
-      <c r="P22" t="n">
-        <v/>
-      </c>
-      <c r="Q22" t="n">
-        <v/>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1972,18 +1700,6 @@
       <c r="M23" t="n">
         <v>2022</v>
       </c>
-      <c r="N23" t="n">
-        <v/>
-      </c>
-      <c r="O23" t="n">
-        <v/>
-      </c>
-      <c r="P23" t="n">
-        <v/>
-      </c>
-      <c r="Q23" t="n">
-        <v/>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2041,18 +1757,6 @@
       <c r="M24" t="n">
         <v>2022</v>
       </c>
-      <c r="N24" t="n">
-        <v/>
-      </c>
-      <c r="O24" t="n">
-        <v/>
-      </c>
-      <c r="P24" t="n">
-        <v/>
-      </c>
-      <c r="Q24" t="n">
-        <v/>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2108,18 +1812,6 @@
       <c r="M25" t="n">
         <v>2021</v>
       </c>
-      <c r="N25" t="n">
-        <v/>
-      </c>
-      <c r="O25" t="n">
-        <v/>
-      </c>
-      <c r="P25" t="n">
-        <v/>
-      </c>
-      <c r="Q25" t="n">
-        <v/>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2175,18 +1867,6 @@
       <c r="M26" t="n">
         <v>2021</v>
       </c>
-      <c r="N26" t="n">
-        <v/>
-      </c>
-      <c r="O26" t="n">
-        <v/>
-      </c>
-      <c r="P26" t="n">
-        <v/>
-      </c>
-      <c r="Q26" t="n">
-        <v/>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2242,18 +1922,6 @@
       <c r="M27" t="n">
         <v>2021</v>
       </c>
-      <c r="N27" t="n">
-        <v/>
-      </c>
-      <c r="O27" t="n">
-        <v/>
-      </c>
-      <c r="P27" t="n">
-        <v/>
-      </c>
-      <c r="Q27" t="n">
-        <v/>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2309,18 +1977,6 @@
       <c r="M28" t="n">
         <v>2021</v>
       </c>
-      <c r="N28" t="n">
-        <v/>
-      </c>
-      <c r="O28" t="n">
-        <v/>
-      </c>
-      <c r="P28" t="n">
-        <v/>
-      </c>
-      <c r="Q28" t="n">
-        <v/>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2376,18 +2032,6 @@
       <c r="M29" t="n">
         <v>2021</v>
       </c>
-      <c r="N29" t="n">
-        <v/>
-      </c>
-      <c r="O29" t="n">
-        <v/>
-      </c>
-      <c r="P29" t="n">
-        <v/>
-      </c>
-      <c r="Q29" t="n">
-        <v/>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2443,18 +2087,6 @@
       <c r="M30" t="n">
         <v>2021</v>
       </c>
-      <c r="N30" t="n">
-        <v/>
-      </c>
-      <c r="O30" t="n">
-        <v/>
-      </c>
-      <c r="P30" t="n">
-        <v/>
-      </c>
-      <c r="Q30" t="n">
-        <v/>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2510,18 +2142,6 @@
       <c r="M31" t="n">
         <v>2020</v>
       </c>
-      <c r="N31" t="n">
-        <v/>
-      </c>
-      <c r="O31" t="n">
-        <v/>
-      </c>
-      <c r="P31" t="n">
-        <v/>
-      </c>
-      <c r="Q31" t="n">
-        <v/>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2577,18 +2197,6 @@
       <c r="M32" t="n">
         <v>2020</v>
       </c>
-      <c r="N32" t="n">
-        <v/>
-      </c>
-      <c r="O32" t="n">
-        <v/>
-      </c>
-      <c r="P32" t="n">
-        <v/>
-      </c>
-      <c r="Q32" t="n">
-        <v/>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2646,18 +2254,6 @@
       <c r="M33" t="n">
         <v>2019</v>
       </c>
-      <c r="N33" t="n">
-        <v/>
-      </c>
-      <c r="O33" t="n">
-        <v/>
-      </c>
-      <c r="P33" t="n">
-        <v/>
-      </c>
-      <c r="Q33" t="n">
-        <v/>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2713,18 +2309,6 @@
       <c r="M34" t="n">
         <v>2019</v>
       </c>
-      <c r="N34" t="n">
-        <v/>
-      </c>
-      <c r="O34" t="n">
-        <v/>
-      </c>
-      <c r="P34" t="n">
-        <v/>
-      </c>
-      <c r="Q34" t="n">
-        <v/>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2780,18 +2364,6 @@
       <c r="M35" t="n">
         <v>2019</v>
       </c>
-      <c r="N35" t="n">
-        <v/>
-      </c>
-      <c r="O35" t="n">
-        <v/>
-      </c>
-      <c r="P35" t="n">
-        <v/>
-      </c>
-      <c r="Q35" t="n">
-        <v/>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2847,18 +2419,6 @@
       <c r="M36" t="n">
         <v>2019</v>
       </c>
-      <c r="N36" t="n">
-        <v/>
-      </c>
-      <c r="O36" t="n">
-        <v/>
-      </c>
-      <c r="P36" t="n">
-        <v/>
-      </c>
-      <c r="Q36" t="n">
-        <v/>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2914,18 +2474,6 @@
       <c r="M37" t="n">
         <v>2019</v>
       </c>
-      <c r="N37" t="n">
-        <v/>
-      </c>
-      <c r="O37" t="n">
-        <v/>
-      </c>
-      <c r="P37" t="n">
-        <v/>
-      </c>
-      <c r="Q37" t="n">
-        <v/>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2981,18 +2529,6 @@
       <c r="M38" t="n">
         <v>2019</v>
       </c>
-      <c r="N38" t="n">
-        <v/>
-      </c>
-      <c r="O38" t="n">
-        <v/>
-      </c>
-      <c r="P38" t="n">
-        <v/>
-      </c>
-      <c r="Q38" t="n">
-        <v/>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3048,18 +2584,6 @@
       <c r="M39" t="n">
         <v>2019</v>
       </c>
-      <c r="N39" t="n">
-        <v/>
-      </c>
-      <c r="O39" t="n">
-        <v/>
-      </c>
-      <c r="P39" t="n">
-        <v/>
-      </c>
-      <c r="Q39" t="n">
-        <v/>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3115,18 +2639,6 @@
       <c r="M40" t="n">
         <v>2019</v>
       </c>
-      <c r="N40" t="n">
-        <v/>
-      </c>
-      <c r="O40" t="n">
-        <v/>
-      </c>
-      <c r="P40" t="n">
-        <v/>
-      </c>
-      <c r="Q40" t="n">
-        <v/>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3182,18 +2694,6 @@
       <c r="M41" t="n">
         <v>2019</v>
       </c>
-      <c r="N41" t="n">
-        <v/>
-      </c>
-      <c r="O41" t="n">
-        <v/>
-      </c>
-      <c r="P41" t="n">
-        <v/>
-      </c>
-      <c r="Q41" t="n">
-        <v/>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3249,18 +2749,6 @@
       <c r="M42" t="n">
         <v>2019</v>
       </c>
-      <c r="N42" t="n">
-        <v/>
-      </c>
-      <c r="O42" t="n">
-        <v/>
-      </c>
-      <c r="P42" t="n">
-        <v/>
-      </c>
-      <c r="Q42" t="n">
-        <v/>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3316,18 +2804,6 @@
       <c r="M43" t="n">
         <v>2018</v>
       </c>
-      <c r="N43" t="n">
-        <v/>
-      </c>
-      <c r="O43" t="n">
-        <v/>
-      </c>
-      <c r="P43" t="n">
-        <v/>
-      </c>
-      <c r="Q43" t="n">
-        <v/>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3383,18 +2859,6 @@
       <c r="M44" t="n">
         <v>2018</v>
       </c>
-      <c r="N44" t="n">
-        <v/>
-      </c>
-      <c r="O44" t="n">
-        <v/>
-      </c>
-      <c r="P44" t="n">
-        <v/>
-      </c>
-      <c r="Q44" t="n">
-        <v/>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3450,18 +2914,6 @@
       <c r="M45" t="n">
         <v>2018</v>
       </c>
-      <c r="N45" t="n">
-        <v/>
-      </c>
-      <c r="O45" t="n">
-        <v/>
-      </c>
-      <c r="P45" t="n">
-        <v/>
-      </c>
-      <c r="Q45" t="n">
-        <v/>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -3517,18 +2969,6 @@
       <c r="M46" t="n">
         <v>2018</v>
       </c>
-      <c r="N46" t="n">
-        <v/>
-      </c>
-      <c r="O46" t="n">
-        <v/>
-      </c>
-      <c r="P46" t="n">
-        <v/>
-      </c>
-      <c r="Q46" t="n">
-        <v/>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3584,18 +3024,6 @@
       <c r="M47" t="n">
         <v>2018</v>
       </c>
-      <c r="N47" t="n">
-        <v/>
-      </c>
-      <c r="O47" t="n">
-        <v/>
-      </c>
-      <c r="P47" t="n">
-        <v/>
-      </c>
-      <c r="Q47" t="n">
-        <v/>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3651,18 +3079,6 @@
       <c r="M48" t="n">
         <v>2018</v>
       </c>
-      <c r="N48" t="n">
-        <v/>
-      </c>
-      <c r="O48" t="n">
-        <v/>
-      </c>
-      <c r="P48" t="n">
-        <v/>
-      </c>
-      <c r="Q48" t="n">
-        <v/>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3718,18 +3134,6 @@
       <c r="M49" t="n">
         <v>2018</v>
       </c>
-      <c r="N49" t="n">
-        <v/>
-      </c>
-      <c r="O49" t="n">
-        <v/>
-      </c>
-      <c r="P49" t="n">
-        <v/>
-      </c>
-      <c r="Q49" t="n">
-        <v/>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3785,18 +3189,6 @@
       <c r="M50" t="n">
         <v>2018</v>
       </c>
-      <c r="N50" t="n">
-        <v/>
-      </c>
-      <c r="O50" t="n">
-        <v/>
-      </c>
-      <c r="P50" t="n">
-        <v/>
-      </c>
-      <c r="Q50" t="n">
-        <v/>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3852,18 +3244,6 @@
       <c r="M51" t="n">
         <v>2018</v>
       </c>
-      <c r="N51" t="n">
-        <v/>
-      </c>
-      <c r="O51" t="n">
-        <v/>
-      </c>
-      <c r="P51" t="n">
-        <v/>
-      </c>
-      <c r="Q51" t="n">
-        <v/>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3919,18 +3299,6 @@
       <c r="M52" t="n">
         <v>2018</v>
       </c>
-      <c r="N52" t="n">
-        <v/>
-      </c>
-      <c r="O52" t="n">
-        <v/>
-      </c>
-      <c r="P52" t="n">
-        <v/>
-      </c>
-      <c r="Q52" t="n">
-        <v/>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3986,18 +3354,6 @@
       <c r="M53" t="n">
         <v>2018</v>
       </c>
-      <c r="N53" t="n">
-        <v/>
-      </c>
-      <c r="O53" t="n">
-        <v/>
-      </c>
-      <c r="P53" t="n">
-        <v/>
-      </c>
-      <c r="Q53" t="n">
-        <v/>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4053,18 +3409,6 @@
       <c r="M54" t="n">
         <v>2018</v>
       </c>
-      <c r="N54" t="n">
-        <v/>
-      </c>
-      <c r="O54" t="n">
-        <v/>
-      </c>
-      <c r="P54" t="n">
-        <v/>
-      </c>
-      <c r="Q54" t="n">
-        <v/>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -4120,18 +3464,6 @@
       <c r="M55" t="n">
         <v>2017</v>
       </c>
-      <c r="N55" t="n">
-        <v/>
-      </c>
-      <c r="O55" t="n">
-        <v/>
-      </c>
-      <c r="P55" t="n">
-        <v/>
-      </c>
-      <c r="Q55" t="n">
-        <v/>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -4187,18 +3519,6 @@
       <c r="M56" t="n">
         <v>2017</v>
       </c>
-      <c r="N56" t="n">
-        <v/>
-      </c>
-      <c r="O56" t="n">
-        <v/>
-      </c>
-      <c r="P56" t="n">
-        <v/>
-      </c>
-      <c r="Q56" t="n">
-        <v/>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -4254,18 +3574,6 @@
       <c r="M57" t="n">
         <v>2017</v>
       </c>
-      <c r="N57" t="n">
-        <v/>
-      </c>
-      <c r="O57" t="n">
-        <v/>
-      </c>
-      <c r="P57" t="n">
-        <v/>
-      </c>
-      <c r="Q57" t="n">
-        <v/>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -4321,18 +3629,6 @@
       <c r="M58" t="n">
         <v>2017</v>
       </c>
-      <c r="N58" t="n">
-        <v/>
-      </c>
-      <c r="O58" t="n">
-        <v/>
-      </c>
-      <c r="P58" t="n">
-        <v/>
-      </c>
-      <c r="Q58" t="n">
-        <v/>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -4388,18 +3684,6 @@
       <c r="M59" t="n">
         <v>2017</v>
       </c>
-      <c r="N59" t="n">
-        <v/>
-      </c>
-      <c r="O59" t="n">
-        <v/>
-      </c>
-      <c r="P59" t="n">
-        <v/>
-      </c>
-      <c r="Q59" t="n">
-        <v/>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -4455,18 +3739,6 @@
       <c r="M60" t="n">
         <v>2017</v>
       </c>
-      <c r="N60" t="n">
-        <v/>
-      </c>
-      <c r="O60" t="n">
-        <v/>
-      </c>
-      <c r="P60" t="n">
-        <v/>
-      </c>
-      <c r="Q60" t="n">
-        <v/>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -4522,18 +3794,6 @@
       <c r="M61" t="n">
         <v>2017</v>
       </c>
-      <c r="N61" t="n">
-        <v/>
-      </c>
-      <c r="O61" t="n">
-        <v/>
-      </c>
-      <c r="P61" t="n">
-        <v/>
-      </c>
-      <c r="Q61" t="n">
-        <v/>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -4589,18 +3849,6 @@
       <c r="M62" t="n">
         <v>2017</v>
       </c>
-      <c r="N62" t="n">
-        <v/>
-      </c>
-      <c r="O62" t="n">
-        <v/>
-      </c>
-      <c r="P62" t="n">
-        <v/>
-      </c>
-      <c r="Q62" t="n">
-        <v/>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -4656,18 +3904,6 @@
       <c r="M63" t="n">
         <v>2017</v>
       </c>
-      <c r="N63" t="n">
-        <v/>
-      </c>
-      <c r="O63" t="n">
-        <v/>
-      </c>
-      <c r="P63" t="n">
-        <v/>
-      </c>
-      <c r="Q63" t="n">
-        <v/>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -4723,18 +3959,6 @@
       <c r="M64" t="n">
         <v>2017</v>
       </c>
-      <c r="N64" t="n">
-        <v/>
-      </c>
-      <c r="O64" t="n">
-        <v/>
-      </c>
-      <c r="P64" t="n">
-        <v/>
-      </c>
-      <c r="Q64" t="n">
-        <v/>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -4790,18 +4014,6 @@
       <c r="M65" t="n">
         <v>2017</v>
       </c>
-      <c r="N65" t="n">
-        <v/>
-      </c>
-      <c r="O65" t="n">
-        <v/>
-      </c>
-      <c r="P65" t="n">
-        <v/>
-      </c>
-      <c r="Q65" t="n">
-        <v/>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -4857,18 +4069,6 @@
       <c r="M66" t="n">
         <v>2016</v>
       </c>
-      <c r="N66" t="n">
-        <v/>
-      </c>
-      <c r="O66" t="n">
-        <v/>
-      </c>
-      <c r="P66" t="n">
-        <v/>
-      </c>
-      <c r="Q66" t="n">
-        <v/>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -4924,18 +4124,6 @@
       <c r="M67" t="n">
         <v>2016</v>
       </c>
-      <c r="N67" t="n">
-        <v/>
-      </c>
-      <c r="O67" t="n">
-        <v/>
-      </c>
-      <c r="P67" t="n">
-        <v/>
-      </c>
-      <c r="Q67" t="n">
-        <v/>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -4991,18 +4179,6 @@
       <c r="M68" t="n">
         <v>2016</v>
       </c>
-      <c r="N68" t="n">
-        <v/>
-      </c>
-      <c r="O68" t="n">
-        <v/>
-      </c>
-      <c r="P68" t="n">
-        <v/>
-      </c>
-      <c r="Q68" t="n">
-        <v/>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -5058,18 +4234,6 @@
       <c r="M69" t="n">
         <v>2016</v>
       </c>
-      <c r="N69" t="n">
-        <v/>
-      </c>
-      <c r="O69" t="n">
-        <v/>
-      </c>
-      <c r="P69" t="n">
-        <v/>
-      </c>
-      <c r="Q69" t="n">
-        <v/>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -5125,18 +4289,6 @@
       <c r="M70" t="n">
         <v>2016</v>
       </c>
-      <c r="N70" t="n">
-        <v/>
-      </c>
-      <c r="O70" t="n">
-        <v/>
-      </c>
-      <c r="P70" t="n">
-        <v/>
-      </c>
-      <c r="Q70" t="n">
-        <v/>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -5192,18 +4344,6 @@
       <c r="M71" t="n">
         <v>2016</v>
       </c>
-      <c r="N71" t="n">
-        <v/>
-      </c>
-      <c r="O71" t="n">
-        <v/>
-      </c>
-      <c r="P71" t="n">
-        <v/>
-      </c>
-      <c r="Q71" t="n">
-        <v/>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -5260,18 +4400,6 @@
       <c r="M72" t="n">
         <v>2015</v>
       </c>
-      <c r="N72" t="n">
-        <v/>
-      </c>
-      <c r="O72" t="n">
-        <v/>
-      </c>
-      <c r="P72" t="n">
-        <v/>
-      </c>
-      <c r="Q72" t="n">
-        <v/>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -5327,18 +4455,6 @@
       <c r="M73" t="n">
         <v>2015</v>
       </c>
-      <c r="N73" t="n">
-        <v/>
-      </c>
-      <c r="O73" t="n">
-        <v/>
-      </c>
-      <c r="P73" t="n">
-        <v/>
-      </c>
-      <c r="Q73" t="n">
-        <v/>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -5394,18 +4510,6 @@
       <c r="M74" t="n">
         <v>2015</v>
       </c>
-      <c r="N74" t="n">
-        <v/>
-      </c>
-      <c r="O74" t="n">
-        <v/>
-      </c>
-      <c r="P74" t="n">
-        <v/>
-      </c>
-      <c r="Q74" t="n">
-        <v/>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -5461,18 +4565,6 @@
       <c r="M75" t="n">
         <v>2015</v>
       </c>
-      <c r="N75" t="n">
-        <v/>
-      </c>
-      <c r="O75" t="n">
-        <v/>
-      </c>
-      <c r="P75" t="n">
-        <v/>
-      </c>
-      <c r="Q75" t="n">
-        <v/>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -5528,18 +4620,6 @@
       <c r="M76" t="n">
         <v>2015</v>
       </c>
-      <c r="N76" t="n">
-        <v/>
-      </c>
-      <c r="O76" t="n">
-        <v/>
-      </c>
-      <c r="P76" t="n">
-        <v/>
-      </c>
-      <c r="Q76" t="n">
-        <v/>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -5595,18 +4675,6 @@
       <c r="M77" t="n">
         <v>2015</v>
       </c>
-      <c r="N77" t="n">
-        <v/>
-      </c>
-      <c r="O77" t="n">
-        <v/>
-      </c>
-      <c r="P77" t="n">
-        <v/>
-      </c>
-      <c r="Q77" t="n">
-        <v/>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -5662,18 +4730,6 @@
       <c r="M78" t="n">
         <v>2015</v>
       </c>
-      <c r="N78" t="n">
-        <v/>
-      </c>
-      <c r="O78" t="n">
-        <v/>
-      </c>
-      <c r="P78" t="n">
-        <v/>
-      </c>
-      <c r="Q78" t="n">
-        <v/>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -5729,18 +4785,6 @@
       <c r="M79" t="n">
         <v>2014</v>
       </c>
-      <c r="N79" t="n">
-        <v/>
-      </c>
-      <c r="O79" t="n">
-        <v/>
-      </c>
-      <c r="P79" t="n">
-        <v/>
-      </c>
-      <c r="Q79" t="n">
-        <v/>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -5796,18 +4840,6 @@
       <c r="M80" t="n">
         <v>2014</v>
       </c>
-      <c r="N80" t="n">
-        <v/>
-      </c>
-      <c r="O80" t="n">
-        <v/>
-      </c>
-      <c r="P80" t="n">
-        <v/>
-      </c>
-      <c r="Q80" t="n">
-        <v/>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -5863,18 +4895,6 @@
       <c r="M81" t="n">
         <v>2014</v>
       </c>
-      <c r="N81" t="n">
-        <v/>
-      </c>
-      <c r="O81" t="n">
-        <v/>
-      </c>
-      <c r="P81" t="n">
-        <v/>
-      </c>
-      <c r="Q81" t="n">
-        <v/>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -5930,18 +4950,6 @@
       <c r="M82" t="n">
         <v>2014</v>
       </c>
-      <c r="N82" t="n">
-        <v/>
-      </c>
-      <c r="O82" t="n">
-        <v/>
-      </c>
-      <c r="P82" t="n">
-        <v/>
-      </c>
-      <c r="Q82" t="n">
-        <v/>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -5997,18 +5005,6 @@
       <c r="M83" t="n">
         <v>2013</v>
       </c>
-      <c r="N83" t="n">
-        <v/>
-      </c>
-      <c r="O83" t="n">
-        <v/>
-      </c>
-      <c r="P83" t="n">
-        <v/>
-      </c>
-      <c r="Q83" t="n">
-        <v/>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -6065,18 +5061,6 @@
       <c r="M84" t="n">
         <v>2013</v>
       </c>
-      <c r="N84" t="n">
-        <v/>
-      </c>
-      <c r="O84" t="n">
-        <v/>
-      </c>
-      <c r="P84" t="n">
-        <v/>
-      </c>
-      <c r="Q84" t="n">
-        <v/>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -6133,18 +5117,6 @@
       <c r="M85" t="n">
         <v>2013</v>
       </c>
-      <c r="N85" t="n">
-        <v/>
-      </c>
-      <c r="O85" t="n">
-        <v/>
-      </c>
-      <c r="P85" t="n">
-        <v/>
-      </c>
-      <c r="Q85" t="n">
-        <v/>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -6201,18 +5173,6 @@
       <c r="M86" t="n">
         <v>2013</v>
       </c>
-      <c r="N86" t="n">
-        <v/>
-      </c>
-      <c r="O86" t="n">
-        <v/>
-      </c>
-      <c r="P86" t="n">
-        <v/>
-      </c>
-      <c r="Q86" t="n">
-        <v/>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -6268,18 +5228,6 @@
       <c r="M87" t="n">
         <v>2013</v>
       </c>
-      <c r="N87" t="n">
-        <v/>
-      </c>
-      <c r="O87" t="n">
-        <v/>
-      </c>
-      <c r="P87" t="n">
-        <v/>
-      </c>
-      <c r="Q87" t="n">
-        <v/>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -6335,18 +5283,6 @@
       <c r="M88" t="n">
         <v>2012</v>
       </c>
-      <c r="N88" t="n">
-        <v/>
-      </c>
-      <c r="O88" t="n">
-        <v/>
-      </c>
-      <c r="P88" t="n">
-        <v/>
-      </c>
-      <c r="Q88" t="n">
-        <v/>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -6402,18 +5338,6 @@
       <c r="M89" t="n">
         <v>2012</v>
       </c>
-      <c r="N89" t="n">
-        <v/>
-      </c>
-      <c r="O89" t="n">
-        <v/>
-      </c>
-      <c r="P89" t="n">
-        <v/>
-      </c>
-      <c r="Q89" t="n">
-        <v/>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -6469,18 +5393,6 @@
       <c r="M90" t="n">
         <v>2012</v>
       </c>
-      <c r="N90" t="n">
-        <v/>
-      </c>
-      <c r="O90" t="n">
-        <v/>
-      </c>
-      <c r="P90" t="n">
-        <v/>
-      </c>
-      <c r="Q90" t="n">
-        <v/>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -6536,18 +5448,6 @@
       <c r="M91" t="n">
         <v>2012</v>
       </c>
-      <c r="N91" t="n">
-        <v/>
-      </c>
-      <c r="O91" t="n">
-        <v/>
-      </c>
-      <c r="P91" t="n">
-        <v/>
-      </c>
-      <c r="Q91" t="n">
-        <v/>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -6603,18 +5503,6 @@
       <c r="M92" t="n">
         <v>2012</v>
       </c>
-      <c r="N92" t="n">
-        <v/>
-      </c>
-      <c r="O92" t="n">
-        <v/>
-      </c>
-      <c r="P92" t="n">
-        <v/>
-      </c>
-      <c r="Q92" t="n">
-        <v/>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -6670,18 +5558,6 @@
       <c r="M93" t="n">
         <v>2012</v>
       </c>
-      <c r="N93" t="n">
-        <v/>
-      </c>
-      <c r="O93" t="n">
-        <v/>
-      </c>
-      <c r="P93" t="n">
-        <v/>
-      </c>
-      <c r="Q93" t="n">
-        <v/>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -6737,18 +5613,6 @@
       <c r="M94" t="n">
         <v>2012</v>
       </c>
-      <c r="N94" t="n">
-        <v/>
-      </c>
-      <c r="O94" t="n">
-        <v/>
-      </c>
-      <c r="P94" t="n">
-        <v/>
-      </c>
-      <c r="Q94" t="n">
-        <v/>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -6804,18 +5668,6 @@
       <c r="M95" t="n">
         <v>2011</v>
       </c>
-      <c r="N95" t="n">
-        <v/>
-      </c>
-      <c r="O95" t="n">
-        <v/>
-      </c>
-      <c r="P95" t="n">
-        <v/>
-      </c>
-      <c r="Q95" t="n">
-        <v/>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -6871,18 +5723,6 @@
       <c r="M96" t="n">
         <v>2011</v>
       </c>
-      <c r="N96" t="n">
-        <v/>
-      </c>
-      <c r="O96" t="n">
-        <v/>
-      </c>
-      <c r="P96" t="n">
-        <v/>
-      </c>
-      <c r="Q96" t="n">
-        <v/>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -6938,18 +5778,6 @@
       <c r="M97" t="n">
         <v>2011</v>
       </c>
-      <c r="N97" t="n">
-        <v/>
-      </c>
-      <c r="O97" t="n">
-        <v/>
-      </c>
-      <c r="P97" t="n">
-        <v/>
-      </c>
-      <c r="Q97" t="n">
-        <v/>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -7005,18 +5833,6 @@
       <c r="M98" t="n">
         <v>2010</v>
       </c>
-      <c r="N98" t="n">
-        <v/>
-      </c>
-      <c r="O98" t="n">
-        <v/>
-      </c>
-      <c r="P98" t="n">
-        <v/>
-      </c>
-      <c r="Q98" t="n">
-        <v/>
-      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -7072,18 +5888,6 @@
       <c r="M99" t="n">
         <v>2009</v>
       </c>
-      <c r="N99" t="n">
-        <v/>
-      </c>
-      <c r="O99" t="n">
-        <v/>
-      </c>
-      <c r="P99" t="n">
-        <v/>
-      </c>
-      <c r="Q99" t="n">
-        <v/>
-      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -7139,18 +5943,6 @@
       <c r="M100" t="n">
         <v>2009</v>
       </c>
-      <c r="N100" t="n">
-        <v/>
-      </c>
-      <c r="O100" t="n">
-        <v/>
-      </c>
-      <c r="P100" t="n">
-        <v/>
-      </c>
-      <c r="Q100" t="n">
-        <v/>
-      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -7206,18 +5998,6 @@
       <c r="M101" t="n">
         <v>2009</v>
       </c>
-      <c r="N101" t="n">
-        <v/>
-      </c>
-      <c r="O101" t="n">
-        <v/>
-      </c>
-      <c r="P101" t="n">
-        <v/>
-      </c>
-      <c r="Q101" t="n">
-        <v/>
-      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -7273,18 +6053,6 @@
       <c r="M102" t="n">
         <v>2009</v>
       </c>
-      <c r="N102" t="n">
-        <v/>
-      </c>
-      <c r="O102" t="n">
-        <v/>
-      </c>
-      <c r="P102" t="n">
-        <v/>
-      </c>
-      <c r="Q102" t="n">
-        <v/>
-      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -7340,18 +6108,6 @@
       <c r="M103" t="n">
         <v>2008</v>
       </c>
-      <c r="N103" t="n">
-        <v/>
-      </c>
-      <c r="O103" t="n">
-        <v/>
-      </c>
-      <c r="P103" t="n">
-        <v/>
-      </c>
-      <c r="Q103" t="n">
-        <v/>
-      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -7407,18 +6163,6 @@
       <c r="M104" t="n">
         <v>2008</v>
       </c>
-      <c r="N104" t="n">
-        <v/>
-      </c>
-      <c r="O104" t="n">
-        <v/>
-      </c>
-      <c r="P104" t="n">
-        <v/>
-      </c>
-      <c r="Q104" t="n">
-        <v/>
-      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -7474,18 +6218,6 @@
       <c r="M105" t="n">
         <v>2008</v>
       </c>
-      <c r="N105" t="n">
-        <v/>
-      </c>
-      <c r="O105" t="n">
-        <v/>
-      </c>
-      <c r="P105" t="n">
-        <v/>
-      </c>
-      <c r="Q105" t="n">
-        <v/>
-      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -7541,18 +6273,6 @@
       <c r="M106" t="n">
         <v>2007</v>
       </c>
-      <c r="N106" t="n">
-        <v/>
-      </c>
-      <c r="O106" t="n">
-        <v/>
-      </c>
-      <c r="P106" t="n">
-        <v/>
-      </c>
-      <c r="Q106" t="n">
-        <v/>
-      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -7608,18 +6328,6 @@
       <c r="M107" t="n">
         <v>2007</v>
       </c>
-      <c r="N107" t="n">
-        <v/>
-      </c>
-      <c r="O107" t="n">
-        <v/>
-      </c>
-      <c r="P107" t="n">
-        <v/>
-      </c>
-      <c r="Q107" t="n">
-        <v/>
-      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -7675,18 +6383,6 @@
       <c r="M108" t="n">
         <v>2007</v>
       </c>
-      <c r="N108" t="n">
-        <v/>
-      </c>
-      <c r="O108" t="n">
-        <v/>
-      </c>
-      <c r="P108" t="n">
-        <v/>
-      </c>
-      <c r="Q108" t="n">
-        <v/>
-      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -7742,18 +6438,6 @@
       <c r="M109" t="n">
         <v>2007</v>
       </c>
-      <c r="N109" t="n">
-        <v/>
-      </c>
-      <c r="O109" t="n">
-        <v/>
-      </c>
-      <c r="P109" t="n">
-        <v/>
-      </c>
-      <c r="Q109" t="n">
-        <v/>
-      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -7809,18 +6493,6 @@
       <c r="M110" t="n">
         <v>2006</v>
       </c>
-      <c r="N110" t="n">
-        <v/>
-      </c>
-      <c r="O110" t="n">
-        <v/>
-      </c>
-      <c r="P110" t="n">
-        <v/>
-      </c>
-      <c r="Q110" t="n">
-        <v/>
-      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -7876,18 +6548,6 @@
       <c r="M111" t="n">
         <v>2006</v>
       </c>
-      <c r="N111" t="n">
-        <v/>
-      </c>
-      <c r="O111" t="n">
-        <v/>
-      </c>
-      <c r="P111" t="n">
-        <v/>
-      </c>
-      <c r="Q111" t="n">
-        <v/>
-      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -7943,18 +6603,6 @@
       <c r="M112" t="n">
         <v>2006</v>
       </c>
-      <c r="N112" t="n">
-        <v/>
-      </c>
-      <c r="O112" t="n">
-        <v/>
-      </c>
-      <c r="P112" t="n">
-        <v/>
-      </c>
-      <c r="Q112" t="n">
-        <v/>
-      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -8010,18 +6658,6 @@
       <c r="M113" t="n">
         <v>2005</v>
       </c>
-      <c r="N113" t="n">
-        <v/>
-      </c>
-      <c r="O113" t="n">
-        <v/>
-      </c>
-      <c r="P113" t="n">
-        <v/>
-      </c>
-      <c r="Q113" t="n">
-        <v/>
-      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -8077,18 +6713,6 @@
       <c r="M114" t="n">
         <v>2005</v>
       </c>
-      <c r="N114" t="n">
-        <v/>
-      </c>
-      <c r="O114" t="n">
-        <v/>
-      </c>
-      <c r="P114" t="n">
-        <v/>
-      </c>
-      <c r="Q114" t="n">
-        <v/>
-      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -8144,18 +6768,6 @@
       <c r="M115" t="n">
         <v>2004</v>
       </c>
-      <c r="N115" t="n">
-        <v/>
-      </c>
-      <c r="O115" t="n">
-        <v/>
-      </c>
-      <c r="P115" t="n">
-        <v/>
-      </c>
-      <c r="Q115" t="n">
-        <v/>
-      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -8211,18 +6823,6 @@
       <c r="M116" t="n">
         <v>2003</v>
       </c>
-      <c r="N116" t="n">
-        <v/>
-      </c>
-      <c r="O116" t="n">
-        <v/>
-      </c>
-      <c r="P116" t="n">
-        <v/>
-      </c>
-      <c r="Q116" t="n">
-        <v/>
-      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -8278,18 +6878,6 @@
       <c r="M117" t="n">
         <v>2001</v>
       </c>
-      <c r="N117" t="n">
-        <v/>
-      </c>
-      <c r="O117" t="n">
-        <v/>
-      </c>
-      <c r="P117" t="n">
-        <v/>
-      </c>
-      <c r="Q117" t="n">
-        <v/>
-      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -8345,18 +6933,6 @@
       <c r="M118" t="n">
         <v>2000</v>
       </c>
-      <c r="N118" t="n">
-        <v/>
-      </c>
-      <c r="O118" t="n">
-        <v/>
-      </c>
-      <c r="P118" t="n">
-        <v/>
-      </c>
-      <c r="Q118" t="n">
-        <v/>
-      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -8412,18 +6988,6 @@
       <c r="M119" t="n">
         <v>1999</v>
       </c>
-      <c r="N119" t="n">
-        <v/>
-      </c>
-      <c r="O119" t="n">
-        <v/>
-      </c>
-      <c r="P119" t="n">
-        <v/>
-      </c>
-      <c r="Q119" t="n">
-        <v/>
-      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -8479,18 +7043,6 @@
       <c r="M120" t="n">
         <v>1999</v>
       </c>
-      <c r="N120" t="n">
-        <v/>
-      </c>
-      <c r="O120" t="n">
-        <v/>
-      </c>
-      <c r="P120" t="n">
-        <v/>
-      </c>
-      <c r="Q120" t="n">
-        <v/>
-      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -8546,18 +7098,6 @@
       <c r="M121" t="n">
         <v>1999</v>
       </c>
-      <c r="N121" t="n">
-        <v/>
-      </c>
-      <c r="O121" t="n">
-        <v/>
-      </c>
-      <c r="P121" t="n">
-        <v/>
-      </c>
-      <c r="Q121" t="n">
-        <v/>
-      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -8613,18 +7153,6 @@
       <c r="M122" t="n">
         <v>1999</v>
       </c>
-      <c r="N122" t="n">
-        <v/>
-      </c>
-      <c r="O122" t="n">
-        <v/>
-      </c>
-      <c r="P122" t="n">
-        <v/>
-      </c>
-      <c r="Q122" t="n">
-        <v/>
-      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -8680,18 +7208,6 @@
       <c r="M123" t="n">
         <v>1999</v>
       </c>
-      <c r="N123" t="n">
-        <v/>
-      </c>
-      <c r="O123" t="n">
-        <v/>
-      </c>
-      <c r="P123" t="n">
-        <v/>
-      </c>
-      <c r="Q123" t="n">
-        <v/>
-      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -8747,18 +7263,6 @@
       <c r="M124" t="n">
         <v>1998</v>
       </c>
-      <c r="N124" t="n">
-        <v/>
-      </c>
-      <c r="O124" t="n">
-        <v/>
-      </c>
-      <c r="P124" t="n">
-        <v/>
-      </c>
-      <c r="Q124" t="n">
-        <v/>
-      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -8814,18 +7318,6 @@
       <c r="M125" t="n">
         <v>1998</v>
       </c>
-      <c r="N125" t="n">
-        <v/>
-      </c>
-      <c r="O125" t="n">
-        <v/>
-      </c>
-      <c r="P125" t="n">
-        <v/>
-      </c>
-      <c r="Q125" t="n">
-        <v/>
-      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -8881,18 +7373,6 @@
       <c r="M126" t="n">
         <v>1998</v>
       </c>
-      <c r="N126" t="n">
-        <v/>
-      </c>
-      <c r="O126" t="n">
-        <v/>
-      </c>
-      <c r="P126" t="n">
-        <v/>
-      </c>
-      <c r="Q126" t="n">
-        <v/>
-      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -8948,18 +7428,6 @@
       <c r="M127" t="n">
         <v>1997</v>
       </c>
-      <c r="N127" t="n">
-        <v/>
-      </c>
-      <c r="O127" t="n">
-        <v/>
-      </c>
-      <c r="P127" t="n">
-        <v/>
-      </c>
-      <c r="Q127" t="n">
-        <v/>
-      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -9015,18 +7483,6 @@
       <c r="M128" t="n">
         <v>1997</v>
       </c>
-      <c r="N128" t="n">
-        <v/>
-      </c>
-      <c r="O128" t="n">
-        <v/>
-      </c>
-      <c r="P128" t="n">
-        <v/>
-      </c>
-      <c r="Q128" t="n">
-        <v/>
-      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -9082,18 +7538,6 @@
       <c r="M129" t="n">
         <v>1996</v>
       </c>
-      <c r="N129" t="n">
-        <v/>
-      </c>
-      <c r="O129" t="n">
-        <v/>
-      </c>
-      <c r="P129" t="n">
-        <v/>
-      </c>
-      <c r="Q129" t="n">
-        <v/>
-      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -9149,18 +7593,6 @@
       <c r="M130" t="n">
         <v>1995</v>
       </c>
-      <c r="N130" t="n">
-        <v/>
-      </c>
-      <c r="O130" t="n">
-        <v/>
-      </c>
-      <c r="P130" t="n">
-        <v/>
-      </c>
-      <c r="Q130" t="n">
-        <v/>
-      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -9216,18 +7648,6 @@
       <c r="M131" t="n">
         <v>1994</v>
       </c>
-      <c r="N131" t="n">
-        <v/>
-      </c>
-      <c r="O131" t="n">
-        <v/>
-      </c>
-      <c r="P131" t="n">
-        <v/>
-      </c>
-      <c r="Q131" t="n">
-        <v/>
-      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -9283,18 +7703,6 @@
       <c r="M132" t="n">
         <v>1993</v>
       </c>
-      <c r="N132" t="n">
-        <v/>
-      </c>
-      <c r="O132" t="n">
-        <v/>
-      </c>
-      <c r="P132" t="n">
-        <v/>
-      </c>
-      <c r="Q132" t="n">
-        <v/>
-      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -9350,18 +7758,6 @@
       <c r="M133" t="n">
         <v>1993</v>
       </c>
-      <c r="N133" t="n">
-        <v/>
-      </c>
-      <c r="O133" t="n">
-        <v/>
-      </c>
-      <c r="P133" t="n">
-        <v/>
-      </c>
-      <c r="Q133" t="n">
-        <v/>
-      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -9417,18 +7813,6 @@
       <c r="M134" t="n">
         <v>1993</v>
       </c>
-      <c r="N134" t="n">
-        <v/>
-      </c>
-      <c r="O134" t="n">
-        <v/>
-      </c>
-      <c r="P134" t="n">
-        <v/>
-      </c>
-      <c r="Q134" t="n">
-        <v/>
-      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -9484,18 +7868,6 @@
       <c r="M135" t="n">
         <v>1993</v>
       </c>
-      <c r="N135" t="n">
-        <v/>
-      </c>
-      <c r="O135" t="n">
-        <v/>
-      </c>
-      <c r="P135" t="n">
-        <v/>
-      </c>
-      <c r="Q135" t="n">
-        <v/>
-      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -9551,18 +7923,6 @@
       <c r="M136" t="n">
         <v>1992</v>
       </c>
-      <c r="N136" t="n">
-        <v/>
-      </c>
-      <c r="O136" t="n">
-        <v/>
-      </c>
-      <c r="P136" t="n">
-        <v/>
-      </c>
-      <c r="Q136" t="n">
-        <v/>
-      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -9618,18 +7978,6 @@
       <c r="M137" t="n">
         <v>1992</v>
       </c>
-      <c r="N137" t="n">
-        <v/>
-      </c>
-      <c r="O137" t="n">
-        <v/>
-      </c>
-      <c r="P137" t="n">
-        <v/>
-      </c>
-      <c r="Q137" t="n">
-        <v/>
-      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -9685,18 +8033,6 @@
       <c r="M138" t="n">
         <v>1991</v>
       </c>
-      <c r="N138" t="n">
-        <v/>
-      </c>
-      <c r="O138" t="n">
-        <v/>
-      </c>
-      <c r="P138" t="n">
-        <v/>
-      </c>
-      <c r="Q138" t="n">
-        <v/>
-      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -9752,18 +8088,6 @@
       <c r="M139" t="n">
         <v>1991</v>
       </c>
-      <c r="N139" t="n">
-        <v/>
-      </c>
-      <c r="O139" t="n">
-        <v/>
-      </c>
-      <c r="P139" t="n">
-        <v/>
-      </c>
-      <c r="Q139" t="n">
-        <v/>
-      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -9819,18 +8143,6 @@
       <c r="M140" t="n">
         <v>1991</v>
       </c>
-      <c r="N140" t="n">
-        <v/>
-      </c>
-      <c r="O140" t="n">
-        <v/>
-      </c>
-      <c r="P140" t="n">
-        <v/>
-      </c>
-      <c r="Q140" t="n">
-        <v/>
-      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -9886,18 +8198,6 @@
       <c r="M141" t="n">
         <v>1990</v>
       </c>
-      <c r="N141" t="n">
-        <v/>
-      </c>
-      <c r="O141" t="n">
-        <v/>
-      </c>
-      <c r="P141" t="n">
-        <v/>
-      </c>
-      <c r="Q141" t="n">
-        <v/>
-      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -9953,18 +8253,6 @@
       <c r="M142" t="n">
         <v>1989</v>
       </c>
-      <c r="N142" t="n">
-        <v/>
-      </c>
-      <c r="O142" t="n">
-        <v/>
-      </c>
-      <c r="P142" t="n">
-        <v/>
-      </c>
-      <c r="Q142" t="n">
-        <v/>
-      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -10020,18 +8308,6 @@
       <c r="M143" t="n">
         <v>1989</v>
       </c>
-      <c r="N143" t="n">
-        <v/>
-      </c>
-      <c r="O143" t="n">
-        <v/>
-      </c>
-      <c r="P143" t="n">
-        <v/>
-      </c>
-      <c r="Q143" t="n">
-        <v/>
-      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -10087,18 +8363,6 @@
       <c r="M144" t="n">
         <v>1988</v>
       </c>
-      <c r="N144" t="n">
-        <v/>
-      </c>
-      <c r="O144" t="n">
-        <v/>
-      </c>
-      <c r="P144" t="n">
-        <v/>
-      </c>
-      <c r="Q144" t="n">
-        <v/>
-      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -10154,18 +8418,6 @@
       <c r="M145" t="n">
         <v>1987</v>
       </c>
-      <c r="N145" t="n">
-        <v/>
-      </c>
-      <c r="O145" t="n">
-        <v/>
-      </c>
-      <c r="P145" t="n">
-        <v/>
-      </c>
-      <c r="Q145" t="n">
-        <v/>
-      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -10221,18 +8473,6 @@
       <c r="M146" t="n">
         <v>1986</v>
       </c>
-      <c r="N146" t="n">
-        <v/>
-      </c>
-      <c r="O146" t="n">
-        <v/>
-      </c>
-      <c r="P146" t="n">
-        <v/>
-      </c>
-      <c r="Q146" t="n">
-        <v/>
-      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -10288,18 +8528,6 @@
       <c r="M147" t="n">
         <v>1984</v>
       </c>
-      <c r="N147" t="n">
-        <v/>
-      </c>
-      <c r="O147" t="n">
-        <v/>
-      </c>
-      <c r="P147" t="n">
-        <v/>
-      </c>
-      <c r="Q147" t="n">
-        <v/>
-      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -10355,18 +8583,6 @@
       <c r="M148" t="n">
         <v>1984</v>
       </c>
-      <c r="N148" t="n">
-        <v/>
-      </c>
-      <c r="O148" t="n">
-        <v/>
-      </c>
-      <c r="P148" t="n">
-        <v/>
-      </c>
-      <c r="Q148" t="n">
-        <v/>
-      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -10421,18 +8637,6 @@
       </c>
       <c r="M149" t="n">
         <v>1982</v>
-      </c>
-      <c r="N149" t="n">
-        <v/>
-      </c>
-      <c r="O149" t="n">
-        <v/>
-      </c>
-      <c r="P149" t="n">
-        <v/>
-      </c>
-      <c r="Q149" t="n">
-        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>